<commit_message>
Most of Sect.4 done; Revisited chi-square; Sect.5 done.
</commit_message>
<xml_diff>
--- a/[H] Requirements Elicitation/Analysis/Codebook.xlsx
+++ b/[H] Requirements Elicitation/Analysis/Codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lucasjohnston.sharepoint.com/sites/Personal/Gedeelde documenten/Studie/[15] Master Thesis/Requirements Elicitation/Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lucasjohnston.sharepoint.com/sites/Personal/Gedeelde documenten/Studie/[15] Master Thesis/[H] Requirements Elicitation/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{A364B7DB-8BCC-4EA4-8BB4-5A401D6DB048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C33A1637-CC64-4BE6-AABE-E1C88AE792DB}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{A364B7DB-8BCC-4EA4-8BB4-5A401D6DB048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF9E5C1F-9F13-4916-B251-1C4263325A6E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55BB6E57-B906-4DEA-B91A-428A96316E9D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55BB6E57-B906-4DEA-B91A-428A96316E9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Interview Coding" sheetId="2" r:id="rId1"/>
@@ -589,17 +589,17 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
-    <col min="3" max="3" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -621,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -629,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -637,7 +637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -648,7 +648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -659,7 +659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -670,7 +670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -681,7 +681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -692,7 +692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -703,7 +703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -711,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -719,7 +719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -727,7 +727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -735,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -743,7 +743,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -751,7 +751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -762,7 +762,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -773,7 +773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -795,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -806,7 +806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -817,7 +817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -825,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -833,7 +833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -841,7 +841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -849,7 +849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -857,7 +857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -868,7 +868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -876,7 +876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -884,7 +884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -892,7 +892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -900,7 +900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -908,7 +908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -916,7 +916,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -924,7 +924,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -945,14 +945,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>63</v>
       </c>
@@ -963,7 +963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -977,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1077,12 +1077,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1115,15 +1115,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007E3BDA08E1E5A249978B11231DCF019A" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a7ca215021bbdd190a5af84d80b652fc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4a4afeb0-7e72-4d51-8cf1-662855e0da1b" xmlns:ns3="63184760-ab03-4f31-8d05-e57fd1de7cd7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f6025b888d8bdcce249ab03fa1f72" ns2:_="" ns3:_="">
     <xsd:import namespace="4a4afeb0-7e72-4d51-8cf1-662855e0da1b"/>
@@ -1318,6 +1309,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51B0394D-43D3-4C78-A5B4-4409E5AE13B6}">
   <ds:schemaRefs>
@@ -1330,13 +1330,13 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{256CBC2F-2FD1-4B5F-ABA4-1000FD3A6B0D}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35C13A16-3150-410A-99CA-DEE7AFCF7374}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E63CCB2-6B9F-45E4-A2DC-F2D79FB02488}"/>
 </file>
</xml_diff>